<commit_message>
ces: Fix inconsistent category names
</commit_message>
<xml_diff>
--- a/emissions/slca/eieio/ces/IO-CEcrosswalk.xlsx
+++ b/emissions/slca/eieio/ces/IO-CEcrosswalk.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="IO-CEcrosswalk" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet state="visible" name="IO-CEcrosswalk" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr refMode="A1" iterate="false" iterateCount="100" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -22,928 +22,945 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="298">
   <si>
-    <t xml:space="preserve">IO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grain farming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cereals and cereal products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other crop farming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oilseed farming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fats and oils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vegetable and melon farming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fresh vegetables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fruit and tree nut farming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fresh fruits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dairy cattle and milk production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fresh milk and cream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beef cattle ranching and farming, including feedlots and dual-purpose ranching and farming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animal production, except cattle and poultry and eggs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poultry and egg production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eggs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fishing, hunting and trapping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fish and seafood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electric power generation, transmission, and distribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural gas distribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water, sewage and other systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water and other public services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential maintenance and repair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maintenance, repairs, insurance, other expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clay product and refractory manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small appliances, miscellaneous housewares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glass and glass product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cutlery and handtool manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miscellaneous household equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawn and garden equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power-driven handtool manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic computer manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telephone apparatus manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audio and video equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audio and visual equipment and services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watch, clock, and other measuring and controlling device manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lighting fixture manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small electrical appliance manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Household cooking appliance manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Major appliances</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Household refrigerator and home freezer manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Household laundry equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other major household appliance manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automobile manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cars and trucks, new</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motorcycle, bicycle, and parts manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other vehicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upholstered household furniture manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Furniture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nonupholstered wood household furniture manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other household nonupholstered furniture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other furniture related product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sporting and athletic goods manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doll, toy, and game manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pets, toys, hobbies, and playground equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other miscellaneous manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dog and cat food manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other animal food manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flour milling and malt manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miscellaneous foods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soybean and other oilseed processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fats and oils refining and blending</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breakfast cereal manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sugar and confectionery product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sugar and other sweets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frozen food manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processed fruits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fruit and vegetable canning, pickling, and drying</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluid milk and butter manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheese manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other dairy products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dry, condensed, and evaporated dairy product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice cream and frozen dessert manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animal (except poultry) slaughtering, rendering, and processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poultry processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poultry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seafood product preparation and packaging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bread and bakery product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bakery products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cookie, cracker, pasta, and tortilla manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snack food manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coffee and tea manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seasoning and dressing manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other food manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soft drink and ice manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breweries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alcoholic beverages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wineries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distilleries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tobacco product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tobacco products and smoking supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fiber, yarn, and thread mills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Household textiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabric mills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Textile and fabric finishing and fabric coating mills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carpet and rug mills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Floor coverings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curtain and linen mills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other textile product mills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apparel manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boys, 2 to 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stationery product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postage and stationery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanitary paper product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other household products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petroleum refineries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuel oil and other fuels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other petroleum and coal products manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pharmaceutical preparation manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drugs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soap and cleaning compound manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laundry and cleaning supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other plastics product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food and beverage stores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General merchandise stores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other retail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other apparel products and services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transit and ground passenger transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Public and other transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Newspaper publishers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Periodical Publishers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Book publishers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software publishers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cable and other subscription programming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wired telecommunications carriers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telephone services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wireless telecommunications carriers (except satellite)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internet publishing and broadcasting and Web search portals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monetary authorities and depository credit intermediation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage interest and charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insurance agencies, brokerages, and related activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Housing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rented dwellings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automotive equipment rental and leasing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle rental, leases, licenses, and other charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elementary and secondary schools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Junior colleges, colleges, universities, and professional schools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other educational services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offices of physicians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offices of dentists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offices of other health practitioners</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outpatient care centers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home health care services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other ambulatory health care services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nursing and community care facilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Child day care services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Children under 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performing arts companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fees and admissions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spectator sports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Museums, historical sites, zoos, and parks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amusement parks and arcades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other amusement and recreation industries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accommodation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other lodging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full-service restaurants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food away from home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limited-service restaurants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other food and drinking places</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automotive repair and maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maintenance and repairs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal and household goods repair and maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal care services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other household expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dry-cleaning and laundry services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other personal services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postal service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cars and trucks, used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processed vegetables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other meats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nonalcoholic beverages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gasoline and motor oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle finance charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Life and other personal insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other entertainment supplies, equipment, and services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal care products and services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Girls, 2 to 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Men, 16 and over</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Women, 16 and over</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greenhouse, nursery, and floriculture production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coal mining</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other wood product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other concrete product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lime and gypsum product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abrasive product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cut stone and stone product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ground or treated mineral and earth manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steel product manufacturing from purchased steel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turned product and screw, nut, and bolt manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ammunition, arms, ordnance, and accessories manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other fabricated metal manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other industrial machinery manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vending, commercial laundry, and other commercial and service industry machinery manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optical instrument and lens manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photographic and photocopying equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heating equipment (except warm air furnaces) manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air conditioning, refrigeration, and warm air heating equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other general purpose machinery manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer storage device manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer terminals and other computer peripheral equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Broadcast and wireless communications equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other communications equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other electronic component manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Printed circuit assembly (electronic assembly) manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electromedical and electrotherapeutic apparatus manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search, detection, and navigation instruments manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacturing and reproducing magnetic and optical media</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electric lamp bulb and part manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power, distribution, and specialty transformer manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor and generator manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switchgear and switchboard apparatus manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storage battery manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary battery manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other miscellaneous electrical equipment and component manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light truck and utility vehicle manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor vehicle body manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor home manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travel trailer and camper manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor vehicle gasoline engine and engine parts manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor vehicle electrical and electronic equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor vehicle steering, suspension component (except spring), and brake systems manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor vehicle transmission and power train parts manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor vehicle seating and interior trim manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other motor vehicle parts manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aircraft manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boat building</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other transportation equipment manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institutional furniture manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Office furniture and custom architectural woodwork and millwork manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Showcase, partition, shelving, and locker manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surgical and medical instrument manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surgical appliance and supplies manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ophthalmic goods manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jewelry and silverware manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Office supplies (except paper) manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wet corn milling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flavoring syrup and concentrate manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leather and allied product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paper mills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paperboard container manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paper bag and coated and treated paper manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other converted paper product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Printing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other basic inorganic chemical manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other basic organic chemical manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fertilizer manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pesticide and other agricultural chemical manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paint and coating manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adhesive manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toilet preparation manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other chemical product and preparation manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plastics packaging materials and unlaminated film and sheet manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polystyrene foam product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urethane and other foam product (except polystyrene) manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tire manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubber and plastics hoses and belting manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other rubber product manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor vehicle and parts dealers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rail transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Truck transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scenic and sightseeing transportation and support activities for transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directory, mailing list, and other publishers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motion picture and video industries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sound recording industries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radio and television broadcasting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Satellite, telecommunications resellers, and all other telecommunications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">News syndicates, libraries, archives and all other information services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nondepository credit intermediation and related activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insurance carriers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumer goods and general rental centers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photographic services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services to buildings and dwellings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waste management and remediation services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical and diagnostic laboratories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential mental retardation, mental health, substance abuse and other facilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community food, housing, and other relief services, including rehabilitation services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promoters of performing arts and sports and agents for public figures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Independent artists, writers, and performers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gambling industries (except casino hotels)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic and precision equipment repair and maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Death care services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used and secondhand goods</t>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>CES</t>
+  </si>
+  <si>
+    <t>Grain farming</t>
+  </si>
+  <si>
+    <t>Cereals and cereal products</t>
+  </si>
+  <si>
+    <t>Other crop farming</t>
+  </si>
+  <si>
+    <t>Oilseed farming</t>
+  </si>
+  <si>
+    <t>Fats and oils</t>
+  </si>
+  <si>
+    <t>Vegetable and melon farming</t>
+  </si>
+  <si>
+    <t>Fresh vegetables</t>
+  </si>
+  <si>
+    <t>Fruit and tree nut farming</t>
+  </si>
+  <si>
+    <t>Fresh fruits</t>
+  </si>
+  <si>
+    <t>Dairy cattle and milk production</t>
+  </si>
+  <si>
+    <t>Fresh milk and cream</t>
+  </si>
+  <si>
+    <t>Beef cattle ranching and farming, including feedlots and dual-purpose ranching and farming</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>Animal production, except cattle and poultry and eggs</t>
+  </si>
+  <si>
+    <t>Pork</t>
+  </si>
+  <si>
+    <t>Poultry and egg production</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>Fishing, hunting and trapping</t>
+  </si>
+  <si>
+    <t>Fish and seafood</t>
+  </si>
+  <si>
+    <t>Electric power generation, transmission, and distribution</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Natural gas distribution</t>
+  </si>
+  <si>
+    <t>Natural gas</t>
+  </si>
+  <si>
+    <t>Water, sewage and other systems</t>
+  </si>
+  <si>
+    <t>Water and other public services</t>
+  </si>
+  <si>
+    <t>Residential maintenance and repair</t>
+  </si>
+  <si>
+    <t>Maintenance, repairs, insurance, other expenses</t>
+  </si>
+  <si>
+    <t>Clay product and refractory manufacturing</t>
+  </si>
+  <si>
+    <t>Small appliances, miscellaneous housewares</t>
+  </si>
+  <si>
+    <t>Glass and glass product manufacturing</t>
+  </si>
+  <si>
+    <t>Cutlery and handtool manufacturing</t>
+  </si>
+  <si>
+    <t>Miscellaneous household equipment</t>
+  </si>
+  <si>
+    <t>Lawn and garden equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Power-driven handtool manufacturing</t>
+  </si>
+  <si>
+    <t>Electronic computer manufacturing</t>
+  </si>
+  <si>
+    <t>Telephone apparatus manufacturing</t>
+  </si>
+  <si>
+    <t>Audio and video equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Audio and visual equipment and services</t>
+  </si>
+  <si>
+    <t>Watch, clock, and other measuring and controlling device manufacturing</t>
+  </si>
+  <si>
+    <t>Lighting fixture manufacturing</t>
+  </si>
+  <si>
+    <t>Small electrical appliance manufacturing</t>
+  </si>
+  <si>
+    <t>Household cooking appliance manufacturing</t>
+  </si>
+  <si>
+    <t>Major appliances</t>
+  </si>
+  <si>
+    <t>Household refrigerator and home freezer manufacturing</t>
+  </si>
+  <si>
+    <t>Household laundry equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Other major household appliance manufacturing</t>
+  </si>
+  <si>
+    <t>Automobile manufacturing</t>
+  </si>
+  <si>
+    <t>Cars and trucks, new</t>
+  </si>
+  <si>
+    <t>Motorcycle, bicycle, and parts manufacturing</t>
+  </si>
+  <si>
+    <t>Other vehicles</t>
+  </si>
+  <si>
+    <t>Upholstered household furniture manufacturing</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>Nonupholstered wood household furniture manufacturing</t>
+  </si>
+  <si>
+    <t>Other household nonupholstered furniture</t>
+  </si>
+  <si>
+    <t>Other furniture related product manufacturing</t>
+  </si>
+  <si>
+    <t>Sporting and athletic goods manufacturing</t>
+  </si>
+  <si>
+    <t>Doll, toy, and game manufacturing</t>
+  </si>
+  <si>
+    <t>Pets, toys, hobbies, and playground equipment</t>
+  </si>
+  <si>
+    <t>All other miscellaneous manufacturing</t>
+  </si>
+  <si>
+    <t>Medical supplies</t>
+  </si>
+  <si>
+    <t>Dog and cat food manufacturing</t>
+  </si>
+  <si>
+    <t>Other animal food manufacturing</t>
+  </si>
+  <si>
+    <t>Flour milling and malt manufacturing</t>
+  </si>
+  <si>
+    <t>Miscellaneous foods</t>
+  </si>
+  <si>
+    <t>Soybean and other oilseed processing</t>
+  </si>
+  <si>
+    <t>Fats and oils refining and blending</t>
+  </si>
+  <si>
+    <t>Breakfast cereal manufacturing</t>
+  </si>
+  <si>
+    <t>Sugar and confectionery product manufacturing</t>
+  </si>
+  <si>
+    <t>Sugar and other sweets</t>
+  </si>
+  <si>
+    <t>Frozen food manufacturing</t>
+  </si>
+  <si>
+    <t>Processed fruits</t>
+  </si>
+  <si>
+    <t>Fruit and vegetable canning, pickling, and drying</t>
+  </si>
+  <si>
+    <t>Fluid milk and butter manufacturing</t>
+  </si>
+  <si>
+    <t>Cheese manufacturing</t>
+  </si>
+  <si>
+    <t>Other dairy products</t>
+  </si>
+  <si>
+    <t>Dry, condensed, and evaporated dairy product manufacturing</t>
+  </si>
+  <si>
+    <t>Ice cream and frozen dessert manufacturing</t>
+  </si>
+  <si>
+    <t>Animal (except poultry) slaughtering, rendering, and processing</t>
+  </si>
+  <si>
+    <t>Poultry processing</t>
+  </si>
+  <si>
+    <t>Poultry</t>
+  </si>
+  <si>
+    <t>Seafood product preparation and packaging</t>
+  </si>
+  <si>
+    <t>Bread and bakery product manufacturing</t>
+  </si>
+  <si>
+    <t>Bakery products</t>
+  </si>
+  <si>
+    <t>Cookie, cracker, pasta, and tortilla manufacturing</t>
+  </si>
+  <si>
+    <t>Snack food manufacturing</t>
+  </si>
+  <si>
+    <t>Coffee and tea manufacturing</t>
+  </si>
+  <si>
+    <t>Seasoning and dressing manufacturing</t>
+  </si>
+  <si>
+    <t>All other food manufacturing</t>
+  </si>
+  <si>
+    <t>Soft drink and ice manufacturing</t>
+  </si>
+  <si>
+    <t>Breweries</t>
+  </si>
+  <si>
+    <t>Alcoholic beverages</t>
+  </si>
+  <si>
+    <t>Wineries</t>
+  </si>
+  <si>
+    <t>Distilleries</t>
+  </si>
+  <si>
+    <t>Tobacco product manufacturing</t>
+  </si>
+  <si>
+    <t>Tobacco products and smoking supplies</t>
+  </si>
+  <si>
+    <t>Fiber, yarn, and thread mills</t>
+  </si>
+  <si>
+    <t>Household textiles</t>
+  </si>
+  <si>
+    <t>Fabric mills</t>
+  </si>
+  <si>
+    <t>Textile and fabric finishing and fabric coating mills</t>
+  </si>
+  <si>
+    <t>Carpet and rug mills</t>
+  </si>
+  <si>
+    <t>Floor coverings</t>
+  </si>
+  <si>
+    <t>Curtain and linen mills</t>
+  </si>
+  <si>
+    <t>Other textile product mills</t>
+  </si>
+  <si>
+    <t>Apparel manufacturing</t>
+  </si>
+  <si>
+    <t>Boys, 2 to 15</t>
+  </si>
+  <si>
+    <t>Stationery product manufacturing</t>
+  </si>
+  <si>
+    <t>Postage and stationery</t>
+  </si>
+  <si>
+    <t>Sanitary paper product manufacturing</t>
+  </si>
+  <si>
+    <t>Other household products</t>
+  </si>
+  <si>
+    <t>Petroleum refineries</t>
+  </si>
+  <si>
+    <t>Fuel oil and other fuels</t>
+  </si>
+  <si>
+    <t>Other petroleum and coal products manufacturing</t>
+  </si>
+  <si>
+    <t>Pharmaceutical preparation manufacturing</t>
+  </si>
+  <si>
+    <t>Drugs</t>
+  </si>
+  <si>
+    <t>Soap and cleaning compound manufacturing</t>
+  </si>
+  <si>
+    <t>Laundry and cleaning supplies</t>
+  </si>
+  <si>
+    <t>Other plastics product manufacturing</t>
+  </si>
+  <si>
+    <t>Food and beverage stores</t>
+  </si>
+  <si>
+    <t>General merchandise stores</t>
+  </si>
+  <si>
+    <t>Other retail</t>
+  </si>
+  <si>
+    <t>Other apparel products and services</t>
+  </si>
+  <si>
+    <t>Transit and ground passenger transportation</t>
+  </si>
+  <si>
+    <t>Public and other transportation</t>
+  </si>
+  <si>
+    <t>Newspaper publishers</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Periodical Publishers</t>
+  </si>
+  <si>
+    <t>Book publishers</t>
+  </si>
+  <si>
+    <t>Software publishers</t>
+  </si>
+  <si>
+    <t>Cable and other subscription programming</t>
+  </si>
+  <si>
+    <t>Wired telecommunications carriers</t>
+  </si>
+  <si>
+    <t>Telephone services</t>
+  </si>
+  <si>
+    <t>Wireless telecommunications carriers (except satellite)</t>
+  </si>
+  <si>
+    <t>Internet publishing and broadcasting and Web search portals</t>
+  </si>
+  <si>
+    <t>Monetary authorities and depository credit intermediation</t>
+  </si>
+  <si>
+    <t>Mortgage interest and charges</t>
+  </si>
+  <si>
+    <t>Insurance agencies, brokerages, and related activities</t>
+  </si>
+  <si>
+    <t>Health insurance</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Rented dwellings</t>
+  </si>
+  <si>
+    <t>Automotive equipment rental and leasing</t>
+  </si>
+  <si>
+    <t>Vehicle rental, leases, licenses, and other charges</t>
+  </si>
+  <si>
+    <t>Elementary and secondary schools</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Junior colleges, colleges, universities, and professional schools</t>
+  </si>
+  <si>
+    <t>Other educational services</t>
+  </si>
+  <si>
+    <t>Offices of physicians</t>
+  </si>
+  <si>
+    <t>Medical services</t>
+  </si>
+  <si>
+    <t>Offices of dentists</t>
+  </si>
+  <si>
+    <t>Offices of other health practitioners</t>
+  </si>
+  <si>
+    <t>Outpatient care centers</t>
+  </si>
+  <si>
+    <t>Home health care services</t>
+  </si>
+  <si>
+    <t>Other ambulatory health care services</t>
+  </si>
+  <si>
+    <t>Hospitals</t>
+  </si>
+  <si>
+    <t>Nursing and community care facilities</t>
+  </si>
+  <si>
+    <t>Child day care services</t>
+  </si>
+  <si>
+    <t>Children under 2</t>
+  </si>
+  <si>
+    <t>Performing arts companies</t>
+  </si>
+  <si>
+    <t>Fees and admissions</t>
+  </si>
+  <si>
+    <t>Spectator sports</t>
+  </si>
+  <si>
+    <t>Museums, historical sites, zoos, and parks</t>
+  </si>
+  <si>
+    <t>Amusement parks and arcades</t>
+  </si>
+  <si>
+    <t>Other amusement and recreation industries</t>
+  </si>
+  <si>
+    <t>Accommodation</t>
+  </si>
+  <si>
+    <t>Other lodging</t>
+  </si>
+  <si>
+    <t>Full-service restaurants</t>
+  </si>
+  <si>
+    <t>Food away from home</t>
+  </si>
+  <si>
+    <t>Limited-service restaurants</t>
+  </si>
+  <si>
+    <t>All other food and drinking places</t>
+  </si>
+  <si>
+    <t>Automotive repair and maintenance</t>
+  </si>
+  <si>
+    <t>Maintenance and repairs</t>
+  </si>
+  <si>
+    <t>Personal and household goods repair and maintenance</t>
+  </si>
+  <si>
+    <t>Personal care services</t>
+  </si>
+  <si>
+    <t>Other household expenses</t>
+  </si>
+  <si>
+    <t>Dry-cleaning and laundry services</t>
+  </si>
+  <si>
+    <t>Other personal services</t>
+  </si>
+  <si>
+    <t>Postal service</t>
+  </si>
+  <si>
+    <t>Cars and trucks, used</t>
+  </si>
+  <si>
+    <t>Processed vegetables</t>
+  </si>
+  <si>
+    <t>Other meats</t>
+  </si>
+  <si>
+    <t>Nonalcoholic beverages</t>
+  </si>
+  <si>
+    <t>Gasoline and motor oil</t>
+  </si>
+  <si>
+    <t>Vehicle finance charges</t>
+  </si>
+  <si>
+    <t>Life and other personal insurance</t>
+  </si>
+  <si>
+    <t>Other entertainment supplies, equipment, and services</t>
+  </si>
+  <si>
+    <t>Personal care products and services</t>
+  </si>
+  <si>
+    <t>Footwear</t>
+  </si>
+  <si>
+    <t>Vehicle insurance</t>
+  </si>
+  <si>
+    <t>Personal services</t>
+  </si>
+  <si>
+    <t>Girls, 2 to 15</t>
+  </si>
+  <si>
+    <t>Men, 16 and over</t>
+  </si>
+  <si>
+    <t>Women, 16 and over</t>
+  </si>
+  <si>
+    <t>Greenhouse, nursery, and floriculture production</t>
+  </si>
+  <si>
+    <t>Coal mining</t>
+  </si>
+  <si>
+    <t>All other wood product manufacturing</t>
+  </si>
+  <si>
+    <t>Other concrete product manufacturing</t>
+  </si>
+  <si>
+    <t>Lime and gypsum product manufacturing</t>
+  </si>
+  <si>
+    <t>Abrasive product manufacturing</t>
+  </si>
+  <si>
+    <t>Cut stone and stone product manufacturing</t>
+  </si>
+  <si>
+    <t>Ground or treated mineral and earth manufacturing</t>
+  </si>
+  <si>
+    <t>Steel product manufacturing from purchased steel</t>
+  </si>
+  <si>
+    <t>Turned product and screw, nut, and bolt manufacturing</t>
+  </si>
+  <si>
+    <t>Ammunition, arms, ordnance, and accessories manufacturing</t>
+  </si>
+  <si>
+    <t>Other fabricated metal manufacturing</t>
+  </si>
+  <si>
+    <t>Other industrial machinery manufacturing</t>
+  </si>
+  <si>
+    <t>Vending, commercial laundry, and other commercial and service industry machinery manufacturing</t>
+  </si>
+  <si>
+    <t>Optical instrument and lens manufacturing</t>
+  </si>
+  <si>
+    <t>Photographic and photocopying equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Heating equipment (except warm air furnaces) manufacturing</t>
+  </si>
+  <si>
+    <t>Air conditioning, refrigeration, and warm air heating equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Other general purpose machinery manufacturing</t>
+  </si>
+  <si>
+    <t>Computer storage device manufacturing</t>
+  </si>
+  <si>
+    <t>Computer terminals and other computer peripheral equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Broadcast and wireless communications equipment</t>
+  </si>
+  <si>
+    <t>Other communications equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Other electronic component manufacturing</t>
+  </si>
+  <si>
+    <t>Printed circuit assembly (electronic assembly) manufacturing</t>
+  </si>
+  <si>
+    <t>Electromedical and electrotherapeutic apparatus manufacturing</t>
+  </si>
+  <si>
+    <t>Search, detection, and navigation instruments manufacturing</t>
+  </si>
+  <si>
+    <t>Manufacturing and reproducing magnetic and optical media</t>
+  </si>
+  <si>
+    <t>Electric lamp bulb and part manufacturing</t>
+  </si>
+  <si>
+    <t>Power, distribution, and specialty transformer manufacturing</t>
+  </si>
+  <si>
+    <t>Motor and generator manufacturing</t>
+  </si>
+  <si>
+    <t>Switchgear and switchboard apparatus manufacturing</t>
+  </si>
+  <si>
+    <t>Storage battery manufacturing</t>
+  </si>
+  <si>
+    <t>Primary battery manufacturing</t>
+  </si>
+  <si>
+    <t>All other miscellaneous electrical equipment and component manufacturing</t>
+  </si>
+  <si>
+    <t>Light truck and utility vehicle manufacturing</t>
+  </si>
+  <si>
+    <t>Motor vehicle body manufacturing</t>
+  </si>
+  <si>
+    <t>Motor home manufacturing</t>
+  </si>
+  <si>
+    <t>Travel trailer and camper manufacturing</t>
+  </si>
+  <si>
+    <t>Motor vehicle gasoline engine and engine parts manufacturing</t>
+  </si>
+  <si>
+    <t>Motor vehicle electrical and electronic equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Motor vehicle steering, suspension component (except spring), and brake systems manufacturing</t>
+  </si>
+  <si>
+    <t>Motor vehicle transmission and power train parts manufacturing</t>
+  </si>
+  <si>
+    <t>Motor vehicle seating and interior trim manufacturing</t>
+  </si>
+  <si>
+    <t>Other motor vehicle parts manufacturing</t>
+  </si>
+  <si>
+    <t>Aircraft manufacturing</t>
+  </si>
+  <si>
+    <t>Boat building</t>
+  </si>
+  <si>
+    <t>All other transportation equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Institutional furniture manufacturing</t>
+  </si>
+  <si>
+    <t>Office furniture and custom architectural woodwork and millwork manufacturing</t>
+  </si>
+  <si>
+    <t>Showcase, partition, shelving, and locker manufacturing</t>
+  </si>
+  <si>
+    <t>Surgical and medical instrument manufacturing</t>
+  </si>
+  <si>
+    <t>Surgical appliance and supplies manufacturing</t>
+  </si>
+  <si>
+    <t>Ophthalmic goods manufacturing</t>
+  </si>
+  <si>
+    <t>Jewelry and silverware manufacturing</t>
+  </si>
+  <si>
+    <t>Office supplies (except paper) manufacturing</t>
+  </si>
+  <si>
+    <t>Wet corn milling</t>
+  </si>
+  <si>
+    <t>Flavoring syrup and concentrate manufacturing</t>
+  </si>
+  <si>
+    <t>Leather and allied product manufacturing</t>
+  </si>
+  <si>
+    <t>Paper mills</t>
+  </si>
+  <si>
+    <t>Paperboard container manufacturing</t>
+  </si>
+  <si>
+    <t>Paper bag and coated and treated paper manufacturing</t>
+  </si>
+  <si>
+    <t>All other converted paper product manufacturing</t>
+  </si>
+  <si>
+    <t>Printing</t>
+  </si>
+  <si>
+    <t>Other basic inorganic chemical manufacturing</t>
+  </si>
+  <si>
+    <t>Other basic organic chemical manufacturing</t>
+  </si>
+  <si>
+    <t>Fertilizer manufacturing</t>
+  </si>
+  <si>
+    <t>Pesticide and other agricultural chemical manufacturing</t>
+  </si>
+  <si>
+    <t>Paint and coating manufacturing</t>
+  </si>
+  <si>
+    <t>Adhesive manufacturing</t>
+  </si>
+  <si>
+    <t>Toilet preparation manufacturing</t>
+  </si>
+  <si>
+    <t>All other chemical product and preparation manufacturing</t>
+  </si>
+  <si>
+    <t>Plastics packaging materials and unlaminated film and sheet manufacturing</t>
+  </si>
+  <si>
+    <t>Polystyrene foam product manufacturing</t>
+  </si>
+  <si>
+    <t>Urethane and other foam product (except polystyrene) manufacturing</t>
+  </si>
+  <si>
+    <t>Tire manufacturing</t>
+  </si>
+  <si>
+    <t>Rubber and plastics hoses and belting manufacturing</t>
+  </si>
+  <si>
+    <t>Other rubber product manufacturing</t>
+  </si>
+  <si>
+    <t>Motor vehicle and parts dealers</t>
+  </si>
+  <si>
+    <t>Air transportation</t>
+  </si>
+  <si>
+    <t>Rail transportation</t>
+  </si>
+  <si>
+    <t>Water transportation</t>
+  </si>
+  <si>
+    <t>Truck transportation</t>
+  </si>
+  <si>
+    <t>Scenic and sightseeing transportation and support activities for transportation</t>
+  </si>
+  <si>
+    <t>Directory, mailing list, and other publishers</t>
+  </si>
+  <si>
+    <t>Motion picture and video industries</t>
+  </si>
+  <si>
+    <t>Sound recording industries</t>
+  </si>
+  <si>
+    <t>Radio and television broadcasting</t>
+  </si>
+  <si>
+    <t>Satellite, telecommunications resellers, and all other telecommunications</t>
+  </si>
+  <si>
+    <t>News syndicates, libraries, archives and all other information services</t>
+  </si>
+  <si>
+    <t>Nondepository credit intermediation and related activities</t>
+  </si>
+  <si>
+    <t>Insurance carriers</t>
+  </si>
+  <si>
+    <t>Consumer goods and general rental centers</t>
+  </si>
+  <si>
+    <t>Photographic services</t>
+  </si>
+  <si>
+    <t>Services to buildings and dwellings</t>
+  </si>
+  <si>
+    <t>Waste management and remediation services</t>
+  </si>
+  <si>
+    <t>Medical and diagnostic laboratories</t>
+  </si>
+  <si>
+    <t>Residential mental retardation, mental health, substance abuse and other facilities</t>
+  </si>
+  <si>
+    <t>Community food, housing, and other relief services, including rehabilitation services</t>
+  </si>
+  <si>
+    <t>Promoters of performing arts and sports and agents for public figures</t>
+  </si>
+  <si>
+    <t>Independent artists, writers, and performers</t>
+  </si>
+  <si>
+    <t>Gambling industries (except casino hotels)</t>
+  </si>
+  <si>
+    <t>Electronic and precision equipment repair and maintenance</t>
+  </si>
+  <si>
+    <t>Death care services</t>
+  </si>
+  <si>
+    <t>Used and secondhand goods</t>
+  </si>
+  <si>
+    <t>Television, radios, sound equipment</t>
+  </si>
+  <si>
+    <t>Public transportation</t>
+  </si>
+  <si>
+    <t>Publicand other transportation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1" mc:Ignorable="x14ac">
+  <numFmts count="9">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -955,79 +972,81 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B259"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A224" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A237" activeCellId="0" sqref="A237"/>
+    <sheetView topLeftCell="A224" workbookViewId="0" colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" view="normal" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection pane="topLeft" activeCell="C257" sqref="C257" activeCellId="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="59.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col min="1" max="1" width="59.52" customWidth="1"/>
+    <col min="2" max="2" width="45.62" customWidth="1"/>
+    <col min="3" max="1025" width="11.52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -1043,7 +1062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1051,7 +1070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1059,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
@@ -1067,7 +1086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
@@ -1083,7 +1102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="20.85" outlineLevel="0" r="8">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1091,7 +1110,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1099,7 +1118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
@@ -1107,7 +1126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>19</v>
       </c>
@@ -1115,7 +1134,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>21</v>
       </c>
@@ -1123,7 +1142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>23</v>
       </c>
@@ -1131,7 +1150,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>25</v>
       </c>
@@ -1139,7 +1158,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>27</v>
       </c>
@@ -1147,7 +1166,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>29</v>
       </c>
@@ -1155,7 +1174,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>31</v>
       </c>
@@ -1163,7 +1182,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>32</v>
       </c>
@@ -1171,7 +1190,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>34</v>
       </c>
@@ -1179,7 +1198,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>35</v>
       </c>
@@ -1187,7 +1206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>36</v>
       </c>
@@ -1195,7 +1214,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>37</v>
       </c>
@@ -1203,15 +1222,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row ht="12.8" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>40</v>
       </c>
@@ -1219,7 +1241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>41</v>
       </c>
@@ -1227,7 +1249,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>42</v>
       </c>
@@ -1235,7 +1257,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>43</v>
       </c>
@@ -1243,7 +1265,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>45</v>
       </c>
@@ -1251,7 +1273,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>46</v>
       </c>
@@ -1259,7 +1281,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
         <v>47</v>
       </c>
@@ -1267,7 +1289,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
         <v>48</v>
       </c>
@@ -1275,7 +1297,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>50</v>
       </c>
@@ -1283,7 +1305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>52</v>
       </c>
@@ -1291,7 +1313,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>54</v>
       </c>
@@ -1299,7 +1321,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
         <v>55</v>
       </c>
@@ -1307,7 +1329,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
         <v>56</v>
       </c>
@@ -1315,7 +1337,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>57</v>
       </c>
@@ -1323,7 +1345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>58</v>
       </c>
@@ -1331,7 +1353,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>60</v>
       </c>
@@ -1339,7 +1361,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
         <v>62</v>
       </c>
@@ -1347,7 +1369,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
         <v>63</v>
       </c>
@@ -1355,7 +1377,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
         <v>64</v>
       </c>
@@ -1363,7 +1385,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
         <v>66</v>
       </c>
@@ -1371,7 +1393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
         <v>67</v>
       </c>
@@ -1379,7 +1401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
         <v>68</v>
       </c>
@@ -1387,7 +1409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
         <v>69</v>
       </c>
@@ -1395,7 +1417,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
         <v>71</v>
       </c>
@@ -1403,7 +1425,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
         <v>73</v>
       </c>
@@ -1411,7 +1433,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
         <v>74</v>
       </c>
@@ -1419,7 +1441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
         <v>75</v>
       </c>
@@ -1427,7 +1449,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
         <v>77</v>
       </c>
@@ -1435,7 +1457,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
         <v>78</v>
       </c>
@@ -1443,7 +1465,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
         <v>79</v>
       </c>
@@ -1451,7 +1473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
         <v>80</v>
       </c>
@@ -1459,7 +1481,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
         <v>82</v>
       </c>
@@ -1467,7 +1489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
         <v>83</v>
       </c>
@@ -1475,7 +1497,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
         <v>85</v>
       </c>
@@ -1483,7 +1505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
         <v>86</v>
       </c>
@@ -1491,7 +1513,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
         <v>87</v>
       </c>
@@ -1499,7 +1521,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
         <v>88</v>
       </c>
@@ -1507,7 +1529,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
         <v>89</v>
       </c>
@@ -1515,7 +1537,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
         <v>90</v>
       </c>
@@ -1523,7 +1545,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
         <v>91</v>
       </c>
@@ -1531,7 +1553,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
         <v>93</v>
       </c>
@@ -1539,7 +1561,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
         <v>94</v>
       </c>
@@ -1547,7 +1569,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
         <v>95</v>
       </c>
@@ -1555,7 +1577,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
         <v>97</v>
       </c>
@@ -1563,7 +1585,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
         <v>99</v>
       </c>
@@ -1571,7 +1593,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
         <v>100</v>
       </c>
@@ -1579,7 +1601,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
         <v>101</v>
       </c>
@@ -1587,7 +1609,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
         <v>103</v>
       </c>
@@ -1595,7 +1617,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
         <v>104</v>
       </c>
@@ -1603,7 +1625,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
         <v>105</v>
       </c>
@@ -1611,7 +1633,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
         <v>107</v>
       </c>
@@ -1619,7 +1641,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
         <v>109</v>
       </c>
@@ -1627,7 +1649,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
         <v>111</v>
       </c>
@@ -1635,7 +1657,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
         <v>113</v>
       </c>
@@ -1643,7 +1665,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
         <v>114</v>
       </c>
@@ -1651,7 +1673,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
         <v>116</v>
       </c>
@@ -1659,7 +1681,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
         <v>118</v>
       </c>
@@ -1667,7 +1689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
         <v>119</v>
       </c>
@@ -1675,7 +1697,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
         <v>120</v>
       </c>
@@ -1683,7 +1705,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
         <v>121</v>
       </c>
@@ -1691,15 +1713,21 @@
         <v>122</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
         <v>123</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row ht="12.8" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
         <v>125</v>
       </c>
@@ -1707,7 +1735,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
         <v>127</v>
       </c>
@@ -1715,7 +1743,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
         <v>128</v>
       </c>
@@ -1723,23 +1751,29 @@
         <v>126</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
         <v>129</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row ht="12.8" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
         <v>130</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row ht="12.8" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
         <v>131</v>
       </c>
@@ -1747,7 +1781,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
         <v>133</v>
       </c>
@@ -1755,7 +1789,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
         <v>134</v>
       </c>
@@ -1763,7 +1797,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
         <v>135</v>
       </c>
@@ -1771,7 +1805,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
         <v>137</v>
       </c>
@@ -1779,7 +1813,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
         <v>139</v>
       </c>
@@ -1787,7 +1821,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
         <v>141</v>
       </c>
@@ -1795,7 +1829,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
         <v>143</v>
       </c>
@@ -1803,7 +1837,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
         <v>145</v>
       </c>
@@ -1811,7 +1845,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
         <v>146</v>
       </c>
@@ -1819,7 +1853,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="100">
       <c r="A100" s="0" t="s">
         <v>147</v>
       </c>
@@ -1827,7 +1861,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="101">
       <c r="A101" s="0" t="s">
         <v>149</v>
       </c>
@@ -1835,7 +1869,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
         <v>150</v>
       </c>
@@ -1843,7 +1877,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="103">
       <c r="A103" s="0" t="s">
         <v>151</v>
       </c>
@@ -1851,7 +1885,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="104">
       <c r="A104" s="0" t="s">
         <v>152</v>
       </c>
@@ -1859,7 +1893,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="105">
       <c r="A105" s="0" t="s">
         <v>153</v>
       </c>
@@ -1867,7 +1901,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="106">
       <c r="A106" s="0" t="s">
         <v>154</v>
       </c>
@@ -1875,7 +1909,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="107">
       <c r="A107" s="0" t="s">
         <v>155</v>
       </c>
@@ -1883,7 +1917,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="108">
       <c r="A108" s="0" t="s">
         <v>156</v>
       </c>
@@ -1891,7 +1925,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="109">
       <c r="A109" s="0" t="s">
         <v>158</v>
       </c>
@@ -1899,7 +1933,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="110">
       <c r="A110" s="0" t="s">
         <v>160</v>
       </c>
@@ -1907,7 +1941,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="111">
       <c r="A111" s="0" t="s">
         <v>161</v>
       </c>
@@ -1915,7 +1949,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="112">
       <c r="A112" s="0" t="s">
         <v>162</v>
       </c>
@@ -1923,7 +1957,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="113">
       <c r="A113" s="0" t="s">
         <v>163</v>
       </c>
@@ -1931,7 +1965,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="114">
       <c r="A114" s="0" t="s">
         <v>164</v>
       </c>
@@ -1939,7 +1973,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="115">
       <c r="A115" s="0" t="s">
         <v>166</v>
       </c>
@@ -1947,7 +1981,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="116">
       <c r="A116" s="0" t="s">
         <v>168</v>
       </c>
@@ -1955,7 +1989,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="117">
       <c r="A117" s="0" t="s">
         <v>169</v>
       </c>
@@ -1963,7 +1997,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="118">
       <c r="A118" s="0" t="s">
         <v>170</v>
       </c>
@@ -1971,7 +2005,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="119">
       <c r="A119" s="0" t="s">
         <v>172</v>
       </c>
@@ -1979,7 +2013,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="120">
       <c r="A120" s="0" t="s">
         <v>173</v>
       </c>
@@ -1987,7 +2021,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="121">
       <c r="A121" s="0" t="s">
         <v>175</v>
       </c>
@@ -1995,7 +2029,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="122">
       <c r="A122" s="0" t="s">
         <v>176</v>
       </c>
@@ -2003,7 +2037,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="123">
       <c r="A123" s="0" t="s">
         <v>177</v>
       </c>
@@ -2011,7 +2045,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="124">
       <c r="A124" s="0" t="s">
         <v>17</v>
       </c>
@@ -2019,7 +2053,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="125">
       <c r="A125" s="0" t="s">
         <v>32</v>
       </c>
@@ -2027,7 +2061,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="126">
       <c r="A126" s="0" t="s">
         <v>48</v>
       </c>
@@ -2035,7 +2069,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="127">
       <c r="A127" s="0" t="s">
         <v>60</v>
       </c>
@@ -2043,7 +2077,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="128">
       <c r="A128" s="0" t="s">
         <v>71</v>
       </c>
@@ -2051,7 +2085,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="129">
       <c r="A129" s="0" t="s">
         <v>73</v>
       </c>
@@ -2059,7 +2093,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="130">
       <c r="A130" s="0" t="s">
         <v>79</v>
       </c>
@@ -2067,7 +2101,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="131">
       <c r="A131" s="0" t="s">
         <v>87</v>
       </c>
@@ -2075,7 +2109,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="132">
       <c r="A132" s="0" t="s">
         <v>90</v>
       </c>
@@ -2083,7 +2117,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="133">
       <c r="A133" s="0" t="s">
         <v>105</v>
       </c>
@@ -2091,7 +2125,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="134">
       <c r="A134" s="0" t="s">
         <v>111</v>
       </c>
@@ -2099,7 +2133,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="135">
       <c r="A135" s="0" t="s">
         <v>120</v>
       </c>
@@ -2107,7 +2141,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="136">
       <c r="A136" s="0" t="s">
         <v>135</v>
       </c>
@@ -2115,7 +2149,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="137">
       <c r="A137" s="0" t="s">
         <v>137</v>
       </c>
@@ -2123,7 +2157,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="138">
       <c r="A138" s="0" t="s">
         <v>163</v>
       </c>
@@ -2131,7 +2165,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="139">
       <c r="A139" s="0" t="s">
         <v>169</v>
       </c>
@@ -2139,7 +2173,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="140">
       <c r="A140" s="0" t="s">
         <v>173</v>
       </c>
@@ -2147,7 +2181,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="141">
       <c r="A141" s="0" t="s">
         <v>60</v>
       </c>
@@ -2155,7 +2189,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="142">
       <c r="A142" s="0" t="s">
         <v>79</v>
       </c>
@@ -2163,7 +2197,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="143">
       <c r="A143" s="0" t="s">
         <v>105</v>
       </c>
@@ -2171,7 +2205,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="144">
       <c r="A144" s="0" t="s">
         <v>120</v>
       </c>
@@ -2179,7 +2213,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="145">
       <c r="A145" s="0" t="s">
         <v>137</v>
       </c>
@@ -2187,7 +2221,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="146">
       <c r="A146" s="0" t="s">
         <v>173</v>
       </c>
@@ -2195,7 +2229,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="147">
       <c r="A147" s="0" t="s">
         <v>60</v>
       </c>
@@ -2203,7 +2237,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="148">
       <c r="A148" s="0" t="s">
         <v>105</v>
       </c>
@@ -2211,7 +2245,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="149">
       <c r="A149" s="0" t="s">
         <v>120</v>
       </c>
@@ -2219,7 +2253,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="150">
       <c r="A150" s="0" t="s">
         <v>105</v>
       </c>
@@ -2227,7 +2261,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="151">
       <c r="A151" s="0" t="s">
         <v>120</v>
       </c>
@@ -2235,7 +2269,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="152">
       <c r="A152" s="0" t="s">
         <v>105</v>
       </c>
@@ -2243,7 +2277,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="153">
       <c r="A153" s="0" t="s">
         <v>105</v>
       </c>
@@ -2251,7 +2285,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="154">
       <c r="A154" s="1" t="s">
         <v>193</v>
       </c>
@@ -2259,7 +2293,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="155">
       <c r="A155" s="0" t="s">
         <v>194</v>
       </c>
@@ -2267,7 +2301,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="156">
       <c r="A156" s="0" t="s">
         <v>195</v>
       </c>
@@ -2275,7 +2309,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="157">
       <c r="A157" s="0" t="s">
         <v>196</v>
       </c>
@@ -2283,7 +2317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="158">
       <c r="A158" s="0" t="s">
         <v>197</v>
       </c>
@@ -2291,7 +2325,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="159">
       <c r="A159" s="0" t="s">
         <v>198</v>
       </c>
@@ -2299,7 +2333,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="160">
       <c r="A160" s="0" t="s">
         <v>199</v>
       </c>
@@ -2307,7 +2341,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="161">
       <c r="A161" s="0" t="s">
         <v>200</v>
       </c>
@@ -2315,7 +2349,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="162">
       <c r="A162" s="0" t="s">
         <v>201</v>
       </c>
@@ -2323,7 +2357,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="163">
       <c r="A163" s="0" t="s">
         <v>202</v>
       </c>
@@ -2331,7 +2365,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="164">
       <c r="A164" s="0" t="s">
         <v>203</v>
       </c>
@@ -2339,7 +2373,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="165">
       <c r="A165" s="0" t="s">
         <v>204</v>
       </c>
@@ -2347,7 +2381,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="166">
       <c r="A166" s="0" t="s">
         <v>205</v>
       </c>
@@ -2355,7 +2389,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="167">
       <c r="A167" s="0" t="s">
         <v>206</v>
       </c>
@@ -2363,7 +2397,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="168">
       <c r="A168" s="0" t="s">
         <v>207</v>
       </c>
@@ -2371,7 +2405,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="169">
       <c r="A169" s="0" t="s">
         <v>208</v>
       </c>
@@ -2379,7 +2413,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="170">
       <c r="A170" s="0" t="s">
         <v>209</v>
       </c>
@@ -2387,7 +2421,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="171">
       <c r="A171" s="0" t="s">
         <v>210</v>
       </c>
@@ -2395,7 +2429,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="172">
       <c r="A172" s="0" t="s">
         <v>211</v>
       </c>
@@ -2403,7 +2437,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="173">
       <c r="A173" s="0" t="s">
         <v>212</v>
       </c>
@@ -2411,7 +2445,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="174">
       <c r="A174" s="0" t="s">
         <v>213</v>
       </c>
@@ -2419,7 +2453,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="175">
       <c r="A175" s="0" t="s">
         <v>214</v>
       </c>
@@ -2427,7 +2461,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="176">
       <c r="A176" s="0" t="s">
         <v>215</v>
       </c>
@@ -2435,7 +2469,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="177">
       <c r="A177" s="0" t="s">
         <v>216</v>
       </c>
@@ -2443,7 +2477,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="178">
       <c r="A178" s="0" t="s">
         <v>217</v>
       </c>
@@ -2451,7 +2485,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="179">
       <c r="A179" s="0" t="s">
         <v>218</v>
       </c>
@@ -2459,7 +2493,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="180">
       <c r="A180" s="0" t="s">
         <v>219</v>
       </c>
@@ -2467,7 +2501,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="181">
       <c r="A181" s="0" t="s">
         <v>220</v>
       </c>
@@ -2475,7 +2509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="182">
       <c r="A182" s="0" t="s">
         <v>221</v>
       </c>
@@ -2483,7 +2517,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="183">
       <c r="A183" s="0" t="s">
         <v>222</v>
       </c>
@@ -2491,7 +2525,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="184">
       <c r="A184" s="0" t="s">
         <v>223</v>
       </c>
@@ -2499,7 +2533,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="185">
       <c r="A185" s="0" t="s">
         <v>224</v>
       </c>
@@ -2507,7 +2541,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="186">
       <c r="A186" s="0" t="s">
         <v>225</v>
       </c>
@@ -2515,7 +2549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="187">
       <c r="A187" s="0" t="s">
         <v>226</v>
       </c>
@@ -2523,7 +2557,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="188">
       <c r="A188" s="0" t="s">
         <v>227</v>
       </c>
@@ -2531,7 +2565,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="189">
       <c r="A189" s="0" t="s">
         <v>228</v>
       </c>
@@ -2539,7 +2573,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="190">
       <c r="A190" s="0" t="s">
         <v>229</v>
       </c>
@@ -2547,7 +2581,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="191">
       <c r="A191" s="0" t="s">
         <v>230</v>
       </c>
@@ -2555,7 +2589,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="192">
       <c r="A192" s="0" t="s">
         <v>231</v>
       </c>
@@ -2563,7 +2597,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="193">
       <c r="A193" s="0" t="s">
         <v>232</v>
       </c>
@@ -2571,7 +2605,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="194">
       <c r="A194" s="0" t="s">
         <v>233</v>
       </c>
@@ -2579,7 +2613,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="195">
       <c r="A195" s="0" t="s">
         <v>234</v>
       </c>
@@ -2587,7 +2621,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="196">
       <c r="A196" s="0" t="s">
         <v>235</v>
       </c>
@@ -2595,7 +2629,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="197">
       <c r="A197" s="0" t="s">
         <v>236</v>
       </c>
@@ -2603,7 +2637,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="198">
       <c r="A198" s="0" t="s">
         <v>237</v>
       </c>
@@ -2611,7 +2645,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="199">
       <c r="A199" s="0" t="s">
         <v>238</v>
       </c>
@@ -2619,7 +2653,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="200">
       <c r="A200" s="0" t="s">
         <v>239</v>
       </c>
@@ -2627,7 +2661,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="201">
       <c r="A201" s="0" t="s">
         <v>240</v>
       </c>
@@ -2635,7 +2669,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="202">
       <c r="A202" s="0" t="s">
         <v>241</v>
       </c>
@@ -2643,7 +2677,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="203">
       <c r="A203" s="0" t="s">
         <v>242</v>
       </c>
@@ -2651,7 +2685,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="204">
       <c r="A204" s="0" t="s">
         <v>243</v>
       </c>
@@ -2659,7 +2693,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="205">
       <c r="A205" s="0" t="s">
         <v>244</v>
       </c>
@@ -2667,7 +2701,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="206">
       <c r="A206" s="0" t="s">
         <v>245</v>
       </c>
@@ -2675,7 +2709,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="207">
       <c r="A207" s="0" t="s">
         <v>246</v>
       </c>
@@ -2683,7 +2717,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="208">
       <c r="A208" s="0" t="s">
         <v>247</v>
       </c>
@@ -2691,7 +2725,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="209">
       <c r="A209" s="0" t="s">
         <v>248</v>
       </c>
@@ -2699,7 +2733,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="210">
       <c r="A210" s="0" t="s">
         <v>249</v>
       </c>
@@ -2707,7 +2741,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="211">
       <c r="A211" s="0" t="s">
         <v>250</v>
       </c>
@@ -2715,7 +2749,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="212">
       <c r="A212" s="0" t="s">
         <v>251</v>
       </c>
@@ -2723,7 +2757,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="213">
       <c r="A213" s="0" t="s">
         <v>252</v>
       </c>
@@ -2731,7 +2765,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="214">
       <c r="A214" s="0" t="s">
         <v>253</v>
       </c>
@@ -2739,7 +2773,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="215">
       <c r="A215" s="0" t="s">
         <v>254</v>
       </c>
@@ -2747,7 +2781,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="216">
       <c r="A216" s="0" t="s">
         <v>255</v>
       </c>
@@ -2755,7 +2789,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="217">
       <c r="A217" s="0" t="s">
         <v>256</v>
       </c>
@@ -2763,7 +2797,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="218">
       <c r="A218" s="0" t="s">
         <v>257</v>
       </c>
@@ -2771,7 +2805,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="219">
       <c r="A219" s="0" t="s">
         <v>258</v>
       </c>
@@ -2779,7 +2813,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="220">
       <c r="A220" s="0" t="s">
         <v>259</v>
       </c>
@@ -2787,7 +2821,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="221">
       <c r="A221" s="0" t="s">
         <v>260</v>
       </c>
@@ -2795,7 +2829,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="222">
       <c r="A222" s="0" t="s">
         <v>261</v>
       </c>
@@ -2803,7 +2837,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="223">
       <c r="A223" s="0" t="s">
         <v>262</v>
       </c>
@@ -2811,7 +2845,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="224">
       <c r="A224" s="0" t="s">
         <v>263</v>
       </c>
@@ -2819,7 +2853,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="225">
       <c r="A225" s="0" t="s">
         <v>264</v>
       </c>
@@ -2827,7 +2861,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="226">
       <c r="A226" s="0" t="s">
         <v>265</v>
       </c>
@@ -2835,7 +2869,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="227">
       <c r="A227" s="0" t="s">
         <v>266</v>
       </c>
@@ -2843,7 +2877,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="228">
       <c r="A228" s="0" t="s">
         <v>267</v>
       </c>
@@ -2851,7 +2885,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="229">
       <c r="A229" s="0" t="s">
         <v>268</v>
       </c>
@@ -2859,7 +2893,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="230">
       <c r="A230" s="0" t="s">
         <v>269</v>
       </c>
@@ -2867,7 +2901,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="231">
       <c r="A231" s="0" t="s">
         <v>270</v>
       </c>
@@ -2875,7 +2909,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="232">
       <c r="A232" s="0" t="s">
         <v>271</v>
       </c>
@@ -2883,7 +2917,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="233">
       <c r="A233" s="0" t="s">
         <v>272</v>
       </c>
@@ -2891,7 +2925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="234">
       <c r="A234" s="0" t="s">
         <v>273</v>
       </c>
@@ -2899,7 +2933,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="235">
       <c r="A235" s="0" t="s">
         <v>274</v>
       </c>
@@ -2907,7 +2941,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="236">
       <c r="A236" s="0" t="s">
         <v>275</v>
       </c>
@@ -2915,7 +2949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="237">
       <c r="A237" s="0" t="s">
         <v>111</v>
       </c>
@@ -2923,7 +2957,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="238">
       <c r="A238" s="0" t="s">
         <v>276</v>
       </c>
@@ -2931,7 +2965,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="239">
       <c r="A239" s="0" t="s">
         <v>277</v>
       </c>
@@ -2939,7 +2973,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="240">
       <c r="A240" s="0" t="s">
         <v>278</v>
       </c>
@@ -2947,7 +2981,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="241">
       <c r="A241" s="0" t="s">
         <v>279</v>
       </c>
@@ -2955,7 +2989,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="242">
       <c r="A242" s="0" t="s">
         <v>280</v>
       </c>
@@ -2963,7 +2997,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="243">
       <c r="A243" s="0" t="s">
         <v>281</v>
       </c>
@@ -2971,7 +3005,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="244">
       <c r="A244" s="0" t="s">
         <v>282</v>
       </c>
@@ -2979,7 +3013,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="245">
       <c r="A245" s="0" t="s">
         <v>283</v>
       </c>
@@ -2987,7 +3021,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="246">
       <c r="A246" s="0" t="s">
         <v>284</v>
       </c>
@@ -2995,7 +3029,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="247">
       <c r="A247" s="0" t="s">
         <v>285</v>
       </c>
@@ -3003,7 +3037,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="248">
       <c r="A248" s="0" t="s">
         <v>286</v>
       </c>
@@ -3011,7 +3045,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="249">
       <c r="A249" s="0" t="s">
         <v>287</v>
       </c>
@@ -3019,7 +3053,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="250">
       <c r="A250" s="0" t="s">
         <v>288</v>
       </c>
@@ -3027,7 +3061,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="251">
       <c r="A251" s="0" t="s">
         <v>289</v>
       </c>
@@ -3035,7 +3069,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="252">
       <c r="A252" s="0" t="s">
         <v>290</v>
       </c>
@@ -3043,7 +3077,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="253">
       <c r="A253" s="0" t="s">
         <v>291</v>
       </c>
@@ -3051,7 +3085,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="254">
       <c r="A254" s="0" t="s">
         <v>292</v>
       </c>
@@ -3059,7 +3093,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="255">
       <c r="A255" s="0" t="s">
         <v>293</v>
       </c>
@@ -3067,7 +3101,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="256">
       <c r="A256" s="0" t="s">
         <v>294</v>
       </c>
@@ -3075,15 +3109,18 @@
         <v>159</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="257">
       <c r="A257" s="0" t="s">
         <v>295</v>
       </c>
       <c r="B257" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C257" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row ht="12.8" outlineLevel="0" r="258">
       <c r="A258" s="0" t="s">
         <v>296</v>
       </c>
@@ -3091,7 +3128,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row ht="12.8" outlineLevel="0" r="259">
       <c r="A259" s="0" t="s">
         <v>297</v>
       </c>

</xml_diff>

<commit_message>
ces: Add in all ignored sectors
</commit_message>
<xml_diff>
--- a/emissions/slca/eieio/ces/IO-CEcrosswalk.xlsx
+++ b/emissions/slca/eieio/ces/IO-CEcrosswalk.xlsx
@@ -923,6 +923,135 @@
   </si>
   <si>
     <t>Publicand other transportation</t>
+  </si>
+  <si>
+    <t>"Religious organizations"</t>
+  </si>
+  <si>
+    <t>Religious organizations</t>
+  </si>
+  <si>
+    <t>"Legal services"</t>
+  </si>
+  <si>
+    <t>Legal services</t>
+  </si>
+  <si>
+    <t>Accounting, tax preparation, bookkeeping, and payroll services</t>
+  </si>
+  <si>
+    <t>Specialized design services</t>
+  </si>
+  <si>
+    <t>Scientific research and development services</t>
+  </si>
+  <si>
+    <t>Advertising, public relations, and related services</t>
+  </si>
+  <si>
+    <t>Funds, trusts, and other financial vehicles</t>
+  </si>
+  <si>
+    <t>Securities and commodity contracts intermediation and brokerage</t>
+  </si>
+  <si>
+    <t>Other financial investment activities</t>
+  </si>
+  <si>
+    <t>Couriers and messengers</t>
+  </si>
+  <si>
+    <t>Noncomparable imports</t>
+  </si>
+  <si>
+    <t>Private households</t>
+  </si>
+  <si>
+    <t>Other state and local government enterprises</t>
+  </si>
+  <si>
+    <t>Individual and family services</t>
+  </si>
+  <si>
+    <t>Other support services</t>
+  </si>
+  <si>
+    <t>Veterinary services</t>
+  </si>
+  <si>
+    <t>Employment services</t>
+  </si>
+  <si>
+    <t>Business support services</t>
+  </si>
+  <si>
+    <t>Travel arrangement and reservation services</t>
+  </si>
+  <si>
+    <t>Investigation and security services</t>
+  </si>
+  <si>
+    <t>Other real estate</t>
+  </si>
+  <si>
+    <t>Pipeline transportation</t>
+  </si>
+  <si>
+    <t>Support activities for agriculture and forestry</t>
+  </si>
+  <si>
+    <t>Grantmaking, giving, and social advocacy organizations</t>
+  </si>
+  <si>
+    <t>Civic, social, professional, and similar organizations</t>
+  </si>
+  <si>
+    <t>Commercial and industrial machinery and equipment rental and leasing</t>
+  </si>
+  <si>
+    <t>Warehousing and storage</t>
+  </si>
+  <si>
+    <t>Wholesale trade</t>
+  </si>
+  <si>
+    <t>Other nonmetallic mineral mining and quarrying</t>
+  </si>
+  <si>
+    <t>Iron and steel mills and ferroalloy manufacturing</t>
+  </si>
+  <si>
+    <t>Nonferrous metal (except copper and aluminum) rolling, drawing, extruding and alloying</t>
+  </si>
+  <si>
+    <t>Nonferrous metal foundries</t>
+  </si>
+  <si>
+    <t>Crown and closure manufacturing and metal stamping</t>
+  </si>
+  <si>
+    <t>Plate work and fabricated structural product manufacturing</t>
+  </si>
+  <si>
+    <t>Metal can, box, and other metal container (light gauge) manufacturing</t>
+  </si>
+  <si>
+    <t>Hardware manufacturing</t>
+  </si>
+  <si>
+    <t>Spring and wire product manufacturing</t>
+  </si>
+  <si>
+    <t>Office machinery manufacturing</t>
+  </si>
+  <si>
+    <t>Metal cutting and forming machine tool manufacturing</t>
+  </si>
+  <si>
+    <t>Other engine equipment manufacturing</t>
+  </si>
+  <si>
+    <t>Industrial gas manufacturing</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1165,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView topLeftCell="A224" workbookViewId="0" colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" view="normal" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection pane="topLeft" activeCell="C257" sqref="C257" activeCellId="0"/>
+      <selection pane="topLeft" activeCell="C300" sqref="C300" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12"/>
@@ -3136,6 +3265,373 @@
         <v>33</v>
       </c>
     </row>
+    <row r="260">
+      <c r="A260" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B260" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B261" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B262" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B264" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B265" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B266" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B267" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B268" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B269" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B270" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B271" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B273" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B274" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B275" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B276" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B277" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B279" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B280" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B281" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B282" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B283" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B284" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B285" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B286" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B287" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B288" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C288" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="B289" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C289" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B290" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C290" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="B291" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C291" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B292" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C292" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B293" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C293" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B294" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C294" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="B295" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C295" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B296" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C296" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B297" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C297" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B298" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C298" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B299" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C299" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B300" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C300" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
ces: Refactor to include private demand as part of personal consumption
</commit_message>
<xml_diff>
--- a/emissions/slca/eieio/ces/IO-CEcrosswalk.xlsx
+++ b/emissions/slca/eieio/ces/IO-CEcrosswalk.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="347">
   <si>
     <t xml:space="preserve">IO</t>
   </si>
@@ -635,6 +635,18 @@
   </si>
   <si>
     <t xml:space="preserve">Ground or treated mineral and earth manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-family residential structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multifamily residential structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other residential structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architectural, engineering, and related services</t>
   </si>
   <si>
     <t xml:space="preserve">Steel product manufacturing from purchased steel</t>
@@ -1082,10 +1094,11 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1135,16 +1148,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1164,17 +1177,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F300"/>
+  <dimension ref="A1:F304"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B151" activeCellId="0" sqref="B151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A158" activeCellId="0" sqref="A158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="59.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="59.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,7 +1246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1296,16 +1309,16 @@
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1963,16 +1976,16 @@
       <c r="B95" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E95" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F95" s="3" t="s">
+      <c r="F95" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2127,16 +2140,16 @@
       <c r="B114" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E114" s="3" t="s">
+      <c r="E114" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F114" s="3" t="s">
+      <c r="F114" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2179,16 +2192,16 @@
       <c r="B119" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C119" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D119" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="E119" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F119" s="3" t="s">
+      <c r="F119" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2487,16 +2500,16 @@
       <c r="B156" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C156" s="3" t="s">
+      <c r="C156" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D156" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E156" s="3" t="s">
+      <c r="E156" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F156" s="3" t="s">
+      <c r="F156" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2507,16 +2520,16 @@
       <c r="B157" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C157" s="3" t="s">
+      <c r="C157" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D157" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E157" s="3" t="s">
+      <c r="E157" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F157" s="3" t="s">
+      <c r="F157" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2527,16 +2540,16 @@
       <c r="B158" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="C158" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="D158" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E158" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F158" s="3" t="s">
+      <c r="F158" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2547,16 +2560,16 @@
       <c r="B159" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="C159" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D159" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E159" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F159" s="3" t="s">
+      <c r="F159" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2567,16 +2580,16 @@
       <c r="B160" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="C160" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="D160" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E160" s="3" t="s">
+      <c r="E160" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F160" s="3" t="s">
+      <c r="F160" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2587,16 +2600,16 @@
       <c r="B161" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C161" s="3" t="s">
+      <c r="C161" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D161" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E161" s="3" t="s">
+      <c r="E161" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F161" s="3" t="s">
+      <c r="F161" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2605,31 +2618,79 @@
         <v>205</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="s">
+      <c r="A163" s="3" t="s">
         <v>206</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="s">
+      <c r="A164" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="s">
+      <c r="A165" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,7 +2706,7 @@
         <v>210</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,7 +2714,7 @@
         <v>211</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2661,7 +2722,7 @@
         <v>212</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,7 +2738,7 @@
         <v>214</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>49</v>
+        <v>171</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,7 +2746,7 @@
         <v>215</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2693,7 +2754,7 @@
         <v>216</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,7 +2770,7 @@
         <v>218</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2821,7 +2882,7 @@
         <v>232</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,7 +2890,7 @@
         <v>233</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2837,7 +2898,7 @@
         <v>234</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2845,7 +2906,7 @@
         <v>235</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +2930,7 @@
         <v>238</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2877,7 +2938,7 @@
         <v>239</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2901,7 +2962,7 @@
         <v>242</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,7 +2970,7 @@
         <v>243</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,7 +2978,7 @@
         <v>244</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,7 +2986,7 @@
         <v>245</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2933,7 +2994,7 @@
         <v>246</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2941,7 +3002,7 @@
         <v>247</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2949,7 +3010,7 @@
         <v>248</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,7 +3050,7 @@
         <v>253</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2997,7 +3058,7 @@
         <v>254</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3005,7 +3066,7 @@
         <v>255</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>196</v>
+        <v>58</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,7 +3074,7 @@
         <v>256</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3021,7 +3082,7 @@
         <v>257</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3029,7 +3090,7 @@
         <v>258</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3037,7 +3098,7 @@
         <v>259</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>113</v>
+        <v>196</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,7 +3114,7 @@
         <v>261</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3061,7 +3122,7 @@
         <v>262</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,7 +3130,7 @@
         <v>263</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3077,7 +3138,7 @@
         <v>264</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3085,7 +3146,7 @@
         <v>265</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3093,7 +3154,7 @@
         <v>266</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3101,7 +3162,7 @@
         <v>267</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,7 +3194,7 @@
         <v>271</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3141,7 +3202,7 @@
         <v>272</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3149,7 +3210,7 @@
         <v>273</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3157,7 +3218,7 @@
         <v>274</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,7 +3226,7 @@
         <v>275</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3173,7 +3234,7 @@
         <v>276</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,7 +3242,7 @@
         <v>277</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3189,7 +3250,7 @@
         <v>278</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,47 +3258,47 @@
         <v>279</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>116</v>
+        <v>280</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>186</v>
+        <v>37</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>164</v>
+        <v>37</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>283</v>
+        <v>116</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3245,7 +3306,7 @@
         <v>284</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3253,7 +3314,7 @@
         <v>285</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3277,7 +3338,7 @@
         <v>288</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,7 +3346,7 @@
         <v>289</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3293,7 +3354,7 @@
         <v>290</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3301,19 +3362,7 @@
         <v>291</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C249" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D249" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E249" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F249" s="3" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,19 +3370,7 @@
         <v>292</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C250" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D250" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E250" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F250" s="3" t="s">
-        <v>32</v>
+        <v>188</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3341,7 +3378,7 @@
         <v>293</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3349,7 +3386,7 @@
         <v>294</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3357,7 +3394,19 @@
         <v>295</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>153</v>
+        <v>28</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,7 +3414,19 @@
         <v>296</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>164</v>
+        <v>28</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3373,7 +3434,7 @@
         <v>297</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3381,7 +3442,7 @@
         <v>298</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3389,10 +3450,7 @@
         <v>299</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3400,7 +3458,7 @@
         <v>300</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3408,10 +3466,10 @@
         <v>301</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="260" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
         <v>302</v>
       </c>
@@ -3419,39 +3477,42 @@
         <v>164</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
         <v>303</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="262" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
         <v>304</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="263" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="264" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
         <v>306</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
         <v>307</v>
       </c>
@@ -3459,7 +3520,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
         <v>308</v>
       </c>
@@ -3467,7 +3528,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
         <v>309</v>
       </c>
@@ -3475,7 +3536,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
         <v>310</v>
       </c>
@@ -3483,7 +3544,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
         <v>311</v>
       </c>
@@ -3491,7 +3552,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
         <v>312</v>
       </c>
@@ -3499,7 +3560,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
         <v>313</v>
       </c>
@@ -3507,7 +3568,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
         <v>314</v>
       </c>
@@ -3515,7 +3576,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
         <v>315</v>
       </c>
@@ -3523,7 +3584,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
         <v>316</v>
       </c>
@@ -3531,7 +3592,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
         <v>317</v>
       </c>
@@ -3539,7 +3600,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
         <v>318</v>
       </c>
@@ -3547,7 +3608,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
         <v>319</v>
       </c>
@@ -3555,7 +3616,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
         <v>320</v>
       </c>
@@ -3563,7 +3624,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
         <v>321</v>
       </c>
@@ -3576,38 +3637,26 @@
         <v>322</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C280" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D280" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E280" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F280" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="281" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
         <v>323</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="282" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
         <v>324</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="283" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
         <v>325</v>
       </c>
@@ -3615,31 +3664,43 @@
         <v>178</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
         <v>326</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="285" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
         <v>327</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="286" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
         <v>328</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="287" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
         <v>329</v>
       </c>
@@ -3647,51 +3708,39 @@
         <v>178</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
         <v>330</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="289" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
         <v>331</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C289" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="290" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
         <v>332</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
         <v>333</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C291" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
         <v>334</v>
       </c>
@@ -3702,7 +3751,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
         <v>335</v>
       </c>
@@ -3713,7 +3762,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
         <v>336</v>
       </c>
@@ -3724,7 +3773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
         <v>337</v>
       </c>
@@ -3735,7 +3784,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
         <v>338</v>
       </c>
@@ -3746,7 +3795,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
         <v>339</v>
       </c>
@@ -3757,7 +3806,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
         <v>340</v>
       </c>
@@ -3768,7 +3817,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
         <v>341</v>
       </c>
@@ -3779,7 +3828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
         <v>342</v>
       </c>
@@ -3787,6 +3836,50 @@
         <v>49</v>
       </c>
       <c r="C300" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C304" s="1" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
eieio: Fix bug in negative final demand.
Previously domestic final demand was returning negative values in some 
cases.
</commit_message>
<xml_diff>
--- a/emissions/slca/eieio/ces/IO-CEcrosswalk.xlsx
+++ b/emissions/slca/eieio/ces/IO-CEcrosswalk.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="348">
   <si>
     <t xml:space="preserve">IO</t>
   </si>
@@ -1061,6 +1061,9 @@
   </si>
   <si>
     <t xml:space="preserve">Industrial gas manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest of the world adjustment</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1159,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1177,13 +1180,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F304"/>
+  <dimension ref="A1:BU305"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A158" activeCellId="0" sqref="A158"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A281" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B304" activeCellId="0" sqref="B304"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="59.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.62"/>
@@ -3881,6 +3884,227 @@
       </c>
       <c r="C304" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F305" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G305" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H305" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I305" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J305" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K305" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L305" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M305" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="N305" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O305" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P305" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q305" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="R305" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S305" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="T305" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="U305" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="V305" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W305" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X305" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y305" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z305" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA305" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB305" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC305" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD305" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE305" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF305" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AG305" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AH305" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI305" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ305" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK305" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL305" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AM305" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN305" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO305" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP305" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ305" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR305" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS305" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT305" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AU305" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV305" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AW305" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX305" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AY305" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ305" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BA305" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="BB305" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BC305" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD305" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BE305" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF305" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG305" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="BH305" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BI305" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BJ305" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BK305" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL305" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM305" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BN305" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO305" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="BP305" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BQ305" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="BR305" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BS305" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BT305" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BU305" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>